<commit_message>
Update TS 1.2 Padam Input Template.xlsx
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.2 Padam Input Template.xlsx
@@ -4210,7 +4210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4422,6 +4422,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4706,8 +4709,8 @@
   <dimension ref="A1:Y1691"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A590" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X572" sqref="X572:X575"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T1676" sqref="T1676"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39553,7 +39556,7 @@
       <c r="S1194" s="55" t="s">
         <v>1347</v>
       </c>
-      <c r="T1194" s="21" t="s">
+      <c r="T1194" s="76" t="s">
         <v>1358</v>
       </c>
       <c r="X1194" s="23" t="s">

</xml_diff>

<commit_message>
Jatai and veda lectures 30/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.2 Padam Input Template.xlsx
@@ -4793,8 +4793,8 @@
   <dimension ref="A1:W1691"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U1627" sqref="U1627"/>
+      <pane ySplit="1" topLeftCell="A1010" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1014" sqref="S1014"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TS Padam Template edits 29/11/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.2 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.2 Padam Input Template.xlsx
@@ -4924,9 +4924,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W1691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1686" sqref="H1686"/>
+      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="18.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>